<commit_message>
Agregado sistema imagenes a tst
</commit_message>
<xml_diff>
--- a/public/xlsx/scotia.xlsx
+++ b/public/xlsx/scotia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Valora\frontend\public\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8F95CC0-4E0A-4C36-AF3E-933A237AB15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3841558-B82C-4801-B8E8-D2419C53910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1695" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1791,6 +1791,114 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1809,13 +1917,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1833,407 +1947,293 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="34" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2546,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Y57"/>
+  <dimension ref="A2:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2577,1157 +2577,1248 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
     </row>
     <row r="3" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="136"/>
-      <c r="R4" s="136"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
     </row>
     <row r="5" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="59"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
+      <c r="O5" s="141"/>
+      <c r="P5" s="141"/>
+      <c r="Q5" s="141"/>
+      <c r="R5" s="142"/>
     </row>
     <row r="6" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="30"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="53"/>
     </row>
     <row r="7" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="46"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="72"/>
     </row>
     <row r="8" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="26" t="s">
+      <c r="C8" s="51"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="78"/>
     </row>
     <row r="9" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="26" t="s">
+      <c r="C9" s="51"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="42"/>
-      <c r="Y9" s="145"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="75"/>
+      <c r="Y9" s="32"/>
     </row>
     <row r="10" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
     </row>
     <row r="11" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="137" t="s">
+      <c r="B11" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="137"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="147"/>
+      <c r="E11" s="147"/>
+      <c r="F11" s="147"/>
+      <c r="G11" s="147"/>
+      <c r="H11" s="147"/>
+      <c r="I11" s="147"/>
+      <c r="J11" s="147"/>
+      <c r="K11" s="147"/>
+      <c r="L11" s="147"/>
+      <c r="M11" s="147"/>
+      <c r="N11" s="147"/>
+      <c r="O11" s="147"/>
+      <c r="P11" s="147"/>
+      <c r="Q11" s="147"/>
+      <c r="R11" s="147"/>
     </row>
     <row r="12" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="46"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="72"/>
     </row>
     <row r="13" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="33"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="149"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149"/>
+      <c r="M13" s="149"/>
+      <c r="N13" s="149"/>
+      <c r="O13" s="149"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="149"/>
+      <c r="R13" s="150"/>
     </row>
     <row r="14" spans="1:25" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
-      <c r="G14" s="139"/>
-      <c r="H14" s="139"/>
-      <c r="I14" s="139"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="139"/>
-      <c r="L14" s="139"/>
-      <c r="M14" s="139"/>
-      <c r="N14" s="139"/>
-      <c r="O14" s="139"/>
-      <c r="P14" s="139"/>
-      <c r="Q14" s="139"/>
-      <c r="R14" s="140"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="153"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="153"/>
+      <c r="H14" s="153"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="153"/>
+      <c r="N14" s="153"/>
+      <c r="O14" s="153"/>
+      <c r="P14" s="153"/>
+      <c r="Q14" s="153"/>
+      <c r="R14" s="154"/>
     </row>
     <row r="15" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="150" t="s">
+      <c r="H15" s="63"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="151" t="s">
+      <c r="L15" s="61"/>
+      <c r="M15" s="35" t="s">
         <v>81</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="152"/>
-      <c r="P15" s="153"/>
-      <c r="Q15" s="153"/>
-      <c r="R15" s="154"/>
+      <c r="O15" s="136"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="137"/>
+      <c r="R15" s="138"/>
     </row>
     <row r="16" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="61"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
     </row>
     <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="142" t="s">
+      <c r="B17" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="142"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="142"/>
-      <c r="L17" s="142"/>
-      <c r="M17" s="142"/>
-      <c r="N17" s="142"/>
-      <c r="O17" s="142"/>
-      <c r="P17" s="142"/>
-      <c r="Q17" s="142"/>
-      <c r="R17" s="142"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="145"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="145"/>
+      <c r="P17" s="145"/>
+      <c r="Q17" s="145"/>
+      <c r="R17" s="145"/>
     </row>
     <row r="18" spans="1:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="52"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="52"/>
-      <c r="R18" s="52"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="68"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="68"/>
     </row>
     <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29" t="s">
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27" t="s">
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="30"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="53"/>
     </row>
     <row r="20" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29" t="s">
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="30"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="53"/>
     </row>
     <row r="21" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19" t="s">
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17" t="s">
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="20"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="58"/>
     </row>
     <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22" t="s">
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="25"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="40"/>
     </row>
     <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
     </row>
     <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="141"/>
-      <c r="F24" s="141"/>
-      <c r="G24" s="141"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="141"/>
-      <c r="L24" s="141"/>
-      <c r="M24" s="141"/>
-      <c r="N24" s="141"/>
-      <c r="O24" s="141"/>
-      <c r="P24" s="141"/>
-      <c r="Q24" s="141"/>
-      <c r="R24" s="141"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
     </row>
     <row r="25" spans="1:18" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="146"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="146"/>
-      <c r="J25" s="146"/>
-      <c r="K25" s="146"/>
-      <c r="L25" s="146"/>
-      <c r="M25" s="146"/>
-      <c r="N25" s="146"/>
-      <c r="O25" s="146"/>
-      <c r="P25" s="146"/>
-      <c r="Q25" s="146"/>
-      <c r="R25" s="146"/>
-    </row>
-    <row r="26" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="147" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+    </row>
+    <row r="26" spans="1:18" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+    </row>
+    <row r="27" spans="1:18" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="33"/>
+    </row>
+    <row r="28" spans="1:18" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+    </row>
+    <row r="29" spans="1:18" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
+    </row>
+    <row r="30" spans="1:18" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="33"/>
+    </row>
+    <row r="31" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="147"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
-      <c r="F26" s="147"/>
-      <c r="G26" s="147"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="147"/>
-      <c r="J26" s="147"/>
-      <c r="K26" s="147"/>
-      <c r="L26" s="147"/>
-      <c r="M26" s="147"/>
-      <c r="N26" s="147"/>
-      <c r="O26" s="147"/>
-      <c r="P26" s="147"/>
-      <c r="Q26" s="147"/>
-      <c r="R26" s="147"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="143" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="144"/>
-      <c r="D27" s="65" t="s">
+      <c r="C32" s="81"/>
+      <c r="D32" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="68" t="s">
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="K27" s="69"/>
-      <c r="L27" s="70" t="s">
+      <c r="K32" s="91"/>
+      <c r="L32" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="M27" s="71"/>
-      <c r="N27" s="71"/>
-      <c r="O27" s="71"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="72"/>
-    </row>
-    <row r="28" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="143" t="s">
+      <c r="M32" s="93"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="93"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="94"/>
+    </row>
+    <row r="33" spans="1:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="144"/>
-      <c r="D28" s="73" t="s">
+      <c r="C33" s="81"/>
+      <c r="D33" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="76" t="s">
+      <c r="E33" s="114"/>
+      <c r="F33" s="114"/>
+      <c r="G33" s="114"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="115"/>
+      <c r="J33" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="K28" s="77"/>
-      <c r="L28" s="78" t="s">
+      <c r="K33" s="117"/>
+      <c r="L33" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="M28" s="79"/>
-      <c r="N28" s="79"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
-    </row>
-    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="64" t="s">
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
+      <c r="P33" s="119"/>
+      <c r="Q33" s="119"/>
+      <c r="R33" s="120"/>
+    </row>
+    <row r="34" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="64" t="s">
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="64" t="s">
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="82"/>
-    </row>
-    <row r="30" spans="1:18" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="83"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="86" t="s">
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+      <c r="O34" s="98"/>
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="86"/>
+    </row>
+    <row r="35" spans="1:19" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="101"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="87"/>
-      <c r="H30" s="88" t="s">
+      <c r="G35" s="9"/>
+      <c r="H35" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="89"/>
-      <c r="J30" s="90" t="s">
+      <c r="I35" s="11"/>
+      <c r="J35" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="K30" s="91"/>
-      <c r="L30" s="92" t="s">
+      <c r="K35" s="13"/>
+      <c r="L35" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="93"/>
-      <c r="N30" s="92" t="s">
+      <c r="M35" s="15"/>
+      <c r="N35" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="O30" s="91"/>
-      <c r="P30" s="94" t="s">
+      <c r="O35" s="13"/>
+      <c r="P35" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="96"/>
-    </row>
-    <row r="31" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="97"/>
-      <c r="C31" s="130"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="64" t="s">
+      <c r="Q35" s="96"/>
+      <c r="R35" s="16"/>
+    </row>
+    <row r="36" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="104"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="99" t="s">
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="K31" s="100"/>
-      <c r="L31" s="100"/>
-      <c r="M31" s="100"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="101"/>
-    </row>
-    <row r="32" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="97"/>
-      <c r="C32" s="130"/>
-      <c r="D32" s="130"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="133">
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="89"/>
+    </row>
+    <row r="37" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="104"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="31">
         <v>45742</v>
       </c>
-      <c r="I32" s="132"/>
-      <c r="J32" s="102" t="s">
+      <c r="I37" s="30"/>
+      <c r="J37" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="K32" s="93"/>
-      <c r="L32" s="92" t="s">
+      <c r="K37" s="15"/>
+      <c r="L37" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="M32" s="93"/>
-      <c r="N32" s="92" t="s">
+      <c r="M37" s="15"/>
+      <c r="N37" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="O32" s="91"/>
-      <c r="P32" s="94" t="s">
+      <c r="O37" s="13"/>
+      <c r="P37" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="96"/>
-    </row>
-    <row r="33" spans="1:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="97"/>
-      <c r="C33" s="130"/>
-      <c r="D33" s="130"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="64" t="s">
+      <c r="Q37" s="96"/>
+      <c r="R37" s="16"/>
+    </row>
+    <row r="38" spans="1:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="104"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="103"/>
-      <c r="H33" s="63" t="s">
+      <c r="G38" s="110"/>
+      <c r="H38" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="82"/>
-      <c r="J33" s="99" t="s">
+      <c r="I38" s="86"/>
+      <c r="J38" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K33" s="100"/>
-      <c r="L33" s="100"/>
-      <c r="M33" s="100"/>
-      <c r="N33" s="100"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="100"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="101"/>
-    </row>
-    <row r="34" spans="1:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="104"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="107">
+      <c r="K38" s="88"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
+      <c r="N38" s="88"/>
+      <c r="O38" s="88"/>
+      <c r="P38" s="88"/>
+      <c r="Q38" s="88"/>
+      <c r="R38" s="89"/>
+    </row>
+    <row r="39" spans="1:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="107"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="18">
         <v>189000</v>
       </c>
-      <c r="G34" s="108" t="s">
+      <c r="G39" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="109">
+      <c r="H39" s="20">
         <v>2100</v>
       </c>
-      <c r="I34" s="110"/>
-      <c r="J34" s="90" t="s">
+      <c r="I39" s="21"/>
+      <c r="J39" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="K34" s="93"/>
-      <c r="L34" s="92" t="s">
+      <c r="K39" s="15"/>
+      <c r="L39" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="M34" s="93"/>
-      <c r="N34" s="92" t="s">
+      <c r="M39" s="15"/>
+      <c r="N39" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="O34" s="91"/>
-      <c r="P34" s="94" t="s">
+      <c r="O39" s="13"/>
+      <c r="P39" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="Q34" s="95"/>
-      <c r="R34" s="96"/>
-    </row>
-    <row r="35" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="64" t="s">
+      <c r="Q39" s="96"/>
+      <c r="R39" s="16"/>
+    </row>
+    <row r="40" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="64" t="s">
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="82"/>
-    </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="125" t="s">
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
+      <c r="P40" s="98"/>
+      <c r="Q40" s="98"/>
+      <c r="R40" s="86"/>
+    </row>
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="127"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="129" t="s">
+      <c r="C41" s="27"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I36" s="114" t="s">
+      <c r="I41" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="J36" s="115" t="s">
+      <c r="J41" s="121" t="s">
         <v>78</v>
       </c>
-      <c r="K36" s="116"/>
-      <c r="L36" s="116"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="116"/>
-      <c r="O36" s="116"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="117"/>
-    </row>
-    <row r="37" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="64" t="s">
+      <c r="K41" s="122"/>
+      <c r="L41" s="122"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="122"/>
+      <c r="O41" s="122"/>
+      <c r="P41" s="122"/>
+      <c r="Q41" s="122"/>
+      <c r="R41" s="123"/>
+    </row>
+    <row r="42" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="119"/>
-      <c r="L37" s="119"/>
-      <c r="M37" s="119"/>
-      <c r="N37" s="119"/>
-      <c r="O37" s="119"/>
-      <c r="P37" s="119"/>
-      <c r="Q37" s="119"/>
-      <c r="R37" s="120"/>
-    </row>
-    <row r="38" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="111" t="s">
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="124"/>
+      <c r="K42" s="125"/>
+      <c r="L42" s="125"/>
+      <c r="M42" s="125"/>
+      <c r="N42" s="125"/>
+      <c r="O42" s="125"/>
+      <c r="P42" s="125"/>
+      <c r="Q42" s="125"/>
+      <c r="R42" s="126"/>
+    </row>
+    <row r="43" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="130" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="113">
+      <c r="C43" s="131"/>
+      <c r="D43" s="131"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="23">
         <v>90</v>
       </c>
-      <c r="I38" s="114" t="s">
+      <c r="I43" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="J38" s="122"/>
-      <c r="K38" s="123"/>
-      <c r="L38" s="123"/>
-      <c r="M38" s="123"/>
-      <c r="N38" s="123"/>
-      <c r="O38" s="123"/>
-      <c r="P38" s="123"/>
-      <c r="Q38" s="123"/>
-      <c r="R38" s="124"/>
-    </row>
-    <row r="39" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="52"/>
-      <c r="S39" s="52"/>
-    </row>
-    <row r="40" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="148" t="s">
+      <c r="J43" s="127"/>
+      <c r="K43" s="128"/>
+      <c r="L43" s="128"/>
+      <c r="M43" s="128"/>
+      <c r="N43" s="128"/>
+      <c r="O43" s="128"/>
+      <c r="P43" s="128"/>
+      <c r="Q43" s="128"/>
+      <c r="R43" s="129"/>
+    </row>
+    <row r="44" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="68"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="68"/>
+      <c r="J44" s="68"/>
+      <c r="K44" s="68"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="68"/>
+      <c r="N44" s="68"/>
+      <c r="O44" s="68"/>
+      <c r="P44" s="68"/>
+      <c r="Q44" s="68"/>
+      <c r="R44" s="68"/>
+      <c r="S44" s="68"/>
+    </row>
+    <row r="45" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="148"/>
-      <c r="D40" s="148"/>
-      <c r="E40" s="148"/>
-      <c r="F40" s="148"/>
-      <c r="G40" s="148"/>
-      <c r="H40" s="148"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="148"/>
-      <c r="K40" s="148"/>
-      <c r="L40" s="148"/>
-      <c r="M40" s="148"/>
-      <c r="N40" s="148"/>
-      <c r="O40" s="148"/>
-      <c r="P40" s="148"/>
-      <c r="Q40" s="148"/>
-      <c r="R40" s="148"/>
-    </row>
-    <row r="41" spans="1:19" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="131"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="131"/>
-      <c r="E41" s="131"/>
-      <c r="F41" s="131"/>
-      <c r="G41" s="131"/>
-      <c r="H41" s="131"/>
-      <c r="I41" s="131"/>
-      <c r="J41" s="131"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="131"/>
-      <c r="M41" s="131"/>
-      <c r="N41" s="131"/>
-      <c r="O41" s="131"/>
-      <c r="P41" s="131"/>
-      <c r="Q41" s="131"/>
-      <c r="R41" s="131"/>
-    </row>
-    <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="62" t="s">
+      <c r="C45" s="111"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="111"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="111"/>
+      <c r="N45" s="111"/>
+      <c r="O45" s="111"/>
+      <c r="P45" s="111"/>
+      <c r="Q45" s="111"/>
+      <c r="R45" s="111"/>
+    </row>
+    <row r="46" spans="1:19" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="112"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
+      <c r="K46" s="112"/>
+      <c r="L46" s="112"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
+      <c r="P46" s="112"/>
+      <c r="Q46" s="112"/>
+      <c r="R46" s="112"/>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62"/>
-      <c r="N42" s="62"/>
-      <c r="O42" s="62"/>
-      <c r="P42" s="62"/>
-      <c r="Q42" s="62"/>
-      <c r="R42" s="62"/>
-    </row>
-    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="4" t="s">
+      <c r="C47" s="132"/>
+      <c r="D47" s="132"/>
+      <c r="E47" s="132"/>
+      <c r="F47" s="132"/>
+      <c r="G47" s="132"/>
+      <c r="H47" s="132"/>
+      <c r="I47" s="132"/>
+      <c r="J47" s="132"/>
+      <c r="K47" s="132"/>
+      <c r="L47" s="132"/>
+      <c r="M47" s="132"/>
+      <c r="N47" s="132"/>
+      <c r="O47" s="132"/>
+      <c r="P47" s="132"/>
+      <c r="Q47" s="132"/>
+      <c r="R47" s="132"/>
+    </row>
+    <row r="48" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="13" t="s">
+      <c r="C48" s="43"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="13" t="s">
+      <c r="I48" s="134"/>
+      <c r="J48" s="134"/>
+      <c r="K48" s="135"/>
+      <c r="L48" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="7" t="s">
+      <c r="M48" s="134"/>
+      <c r="N48" s="134"/>
+      <c r="O48" s="134"/>
+      <c r="P48" s="135"/>
+    </row>
+    <row r="49" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="7" t="s">
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="9"/>
-    </row>
-    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="44"/>
+      <c r="P49" s="45"/>
+    </row>
+    <row r="50" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="7" t="s">
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="9"/>
-    </row>
-    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="10" t="s">
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="44"/>
+      <c r="P50" s="45"/>
+    </row>
+    <row r="51" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="10" t="s">
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="12"/>
-    </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="149" t="s">
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="48"/>
+    </row>
+    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="149"/>
-      <c r="D47" s="149"/>
-      <c r="E47" s="149"/>
-      <c r="F47" s="149"/>
-      <c r="G47" s="149"/>
-      <c r="H47" s="149"/>
-      <c r="I47" s="149"/>
-      <c r="J47" s="149"/>
-      <c r="K47" s="149"/>
-      <c r="L47" s="149"/>
-      <c r="M47" s="149"/>
-      <c r="N47" s="149"/>
-      <c r="O47" s="149"/>
-      <c r="P47" s="149"/>
-      <c r="Q47" s="149"/>
-    </row>
-    <row r="48" spans="1:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="52"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B49" s="3" t="s">
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="42"/>
+      <c r="P52" s="42"/>
+      <c r="Q52" s="42"/>
+    </row>
+    <row r="53" spans="1:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="68"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="68"/>
+      <c r="E53" s="68"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="68"/>
+      <c r="I53" s="68"/>
+      <c r="J53" s="68"/>
+      <c r="K53" s="68"/>
+      <c r="L53" s="68"/>
+      <c r="M53" s="68"/>
+      <c r="N53" s="68"/>
+      <c r="O53" s="68"/>
+      <c r="P53" s="68"/>
+      <c r="Q53" s="68"/>
+      <c r="R53" s="68"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L51" s="5" t="s">
+    <row r="56" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L56" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="M52" s="6" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M57" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="L53" t="s">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="A18:R18"/>
-    <mergeCell ref="B4:R4"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="D6:J6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D5:R5"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H44:P44"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B42:R42"/>
-    <mergeCell ref="L43:P43"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="B40:R40"/>
-    <mergeCell ref="B41:R41"/>
-    <mergeCell ref="A39:S39"/>
-    <mergeCell ref="A48:R48"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:R28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:R33"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:R27"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="J36:R38"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="J31:R31"/>
-    <mergeCell ref="B30:E34"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="J35:R35"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="J29:R29"/>
     <mergeCell ref="B17:R17"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B16:R16"/>
-    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:R12"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:R14"/>
+    <mergeCell ref="B47:R47"/>
+    <mergeCell ref="L48:P48"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="A18:R18"/>
+    <mergeCell ref="B45:R45"/>
+    <mergeCell ref="B46:R46"/>
+    <mergeCell ref="A44:S44"/>
+    <mergeCell ref="A53:R53"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="J41:R43"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="J40:R40"/>
+    <mergeCell ref="H49:P49"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B35:E39"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="J34:R34"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J36:R36"/>
     <mergeCell ref="A10:S10"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="B7:C7"/>
@@ -3741,13 +3832,9 @@
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:R9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:R12"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:R13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:R14"/>
+    <mergeCell ref="B4:R4"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="D6:J6"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="G15:I15"/>
@@ -3755,6 +3842,7 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="I19:R19"/>
+    <mergeCell ref="B16:R16"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="I20:R20"/>
@@ -3764,12 +3852,19 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="I22:R22"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="B47:Q47"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="H45:P45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="H46:P46"/>
+    <mergeCell ref="B31:R31"/>
+    <mergeCell ref="B52:Q52"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="H50:P50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="H51:P51"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:R38"/>
+    <mergeCell ref="J32:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>